<commit_message>
GPG Configuration - Command
</commit_message>
<xml_diff>
--- a/Computer_Science/Certs_Key/GPG_Command.xlsx
+++ b/Computer_Science/Certs_Key/GPG_Command.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git\KnowTech_Learning\Computer_Science\Certs_Key\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA645D50-C389-4C74-AB65-00AE59D0F0AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F349AAD0-63B8-464C-9960-D3F490A3CD31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="18705" yWindow="13410" windowWidth="21555" windowHeight="13770" xr2:uid="{EA505645-1DBE-4270-8DAB-183FE19AEE0E}"/>
   </bookViews>
@@ -781,10 +781,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CCE60E1-C566-474F-91E9-C22C6FC9CB7F}">
-  <dimension ref="A1:AN47"/>
+  <dimension ref="A1:AN46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P3" sqref="P3"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A27" sqref="A27:XFD27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1515,31 +1515,50 @@
       <c r="Y25" s="6"/>
       <c r="Z25" s="6"/>
     </row>
-    <row r="28" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="O28" s="4" t="s">
+    <row r="27" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="O27" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="P28" s="4"/>
-      <c r="Q28" s="4"/>
-      <c r="R28" s="4"/>
-      <c r="S28" s="4"/>
-      <c r="T28" s="4"/>
-      <c r="U28" s="4"/>
-      <c r="V28" s="4"/>
-      <c r="W28" s="4"/>
-      <c r="X28" s="4"/>
-      <c r="Y28" s="4"/>
-      <c r="Z28" s="4"/>
+      <c r="P27" s="4"/>
+      <c r="Q27" s="4"/>
+      <c r="R27" s="4"/>
+      <c r="S27" s="4"/>
+      <c r="T27" s="4"/>
+      <c r="U27" s="4"/>
+      <c r="V27" s="4"/>
+      <c r="W27" s="4"/>
+      <c r="X27" s="4"/>
+      <c r="Y27" s="4"/>
+      <c r="Z27" s="4"/>
+    </row>
+    <row r="28" spans="1:26" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="O28" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="P28" s="14"/>
+      <c r="Q28" s="15"/>
+      <c r="R28" s="16" t="str">
+        <f>"gpg --keyserver "&amp;$O28&amp;" --send-keys "&amp;$E$1</f>
+        <v>gpg --keyserver hkp://pgp.mit.edu --send-keys 6AD1D8AFEB92668CCE9E3558022117DA20445FA7</v>
+      </c>
+      <c r="S28" s="17"/>
+      <c r="T28" s="17"/>
+      <c r="U28" s="17"/>
+      <c r="V28" s="17"/>
+      <c r="W28" s="17"/>
+      <c r="X28" s="17"/>
+      <c r="Y28" s="17"/>
+      <c r="Z28" s="18"/>
     </row>
     <row r="29" spans="1:26" ht="45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="O29" s="13" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="P29" s="14"/>
       <c r="Q29" s="15"/>
       <c r="R29" s="16" t="str">
         <f>"gpg --keyserver "&amp;$O29&amp;" --send-keys "&amp;$E$1</f>
-        <v>gpg --keyserver hkp://pgp.mit.edu --send-keys 6AD1D8AFEB92668CCE9E3558022117DA20445FA7</v>
+        <v>gpg --keyserver keyring.debian.org --send-keys 6AD1D8AFEB92668CCE9E3558022117DA20445FA7</v>
       </c>
       <c r="S29" s="17"/>
       <c r="T29" s="17"/>
@@ -1552,13 +1571,13 @@
     </row>
     <row r="30" spans="1:26" ht="45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="O30" s="13" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="P30" s="14"/>
       <c r="Q30" s="15"/>
       <c r="R30" s="16" t="str">
         <f>"gpg --keyserver "&amp;$O30&amp;" --send-keys "&amp;$E$1</f>
-        <v>gpg --keyserver keyring.debian.org --send-keys 6AD1D8AFEB92668CCE9E3558022117DA20445FA7</v>
+        <v>gpg --keyserver keyserver.ubuntu.com --send-keys 6AD1D8AFEB92668CCE9E3558022117DA20445FA7</v>
       </c>
       <c r="S30" s="17"/>
       <c r="T30" s="17"/>
@@ -1571,13 +1590,13 @@
     </row>
     <row r="31" spans="1:26" ht="45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="O31" s="13" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="P31" s="14"/>
       <c r="Q31" s="15"/>
       <c r="R31" s="16" t="str">
         <f>"gpg --keyserver "&amp;$O31&amp;" --send-keys "&amp;$E$1</f>
-        <v>gpg --keyserver keyserver.ubuntu.com --send-keys 6AD1D8AFEB92668CCE9E3558022117DA20445FA7</v>
+        <v>gpg --keyserver keys.openpgp.org --send-keys 6AD1D8AFEB92668CCE9E3558022117DA20445FA7</v>
       </c>
       <c r="S31" s="17"/>
       <c r="T31" s="17"/>
@@ -1588,45 +1607,26 @@
       <c r="Y31" s="17"/>
       <c r="Z31" s="18"/>
     </row>
-    <row r="32" spans="1:26" ht="45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="O32" s="13" t="s">
-        <v>34</v>
-      </c>
-      <c r="P32" s="14"/>
-      <c r="Q32" s="15"/>
-      <c r="R32" s="16" t="str">
-        <f>"gpg --keyserver "&amp;$O32&amp;" --send-keys "&amp;$E$1</f>
-        <v>gpg --keyserver keys.openpgp.org --send-keys 6AD1D8AFEB92668CCE9E3558022117DA20445FA7</v>
-      </c>
-      <c r="S32" s="17"/>
-      <c r="T32" s="17"/>
-      <c r="U32" s="17"/>
-      <c r="V32" s="17"/>
-      <c r="W32" s="17"/>
-      <c r="X32" s="17"/>
-      <c r="Y32" s="17"/>
-      <c r="Z32" s="18"/>
-    </row>
-    <row r="34" ht="45" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="36" ht="45" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="33" ht="45" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="35" ht="45" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="43" ht="45" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="44" ht="45" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="45" ht="45" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="46" ht="45" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="47" ht="45" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="57">
     <mergeCell ref="O5:Z5"/>
-    <mergeCell ref="O32:Q32"/>
     <mergeCell ref="O31:Q31"/>
+    <mergeCell ref="O30:Q30"/>
+    <mergeCell ref="R28:Z28"/>
     <mergeCell ref="R29:Z29"/>
     <mergeCell ref="R30:Z30"/>
     <mergeCell ref="R31:Z31"/>
-    <mergeCell ref="R32:Z32"/>
     <mergeCell ref="O25:Z25"/>
     <mergeCell ref="A7:L7"/>
     <mergeCell ref="A8:L8"/>
+    <mergeCell ref="O28:Q28"/>
     <mergeCell ref="O29:Q29"/>
-    <mergeCell ref="O30:Q30"/>
     <mergeCell ref="O10:Z10"/>
     <mergeCell ref="O11:Z11"/>
     <mergeCell ref="O12:Z12"/>
@@ -1640,7 +1640,7 @@
     <mergeCell ref="AC11:AN11"/>
     <mergeCell ref="AC14:AN14"/>
     <mergeCell ref="AC15:AN15"/>
-    <mergeCell ref="O28:Z28"/>
+    <mergeCell ref="O27:Z27"/>
     <mergeCell ref="O21:Z21"/>
     <mergeCell ref="O22:Z22"/>
     <mergeCell ref="O23:Z23"/>

</xml_diff>